<commit_message>
middle of lab 6
</commit_message>
<xml_diff>
--- a/lab6/IMU Readings.xlsx
+++ b/lab6/IMU Readings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitlinstanton/Desktop/ece4960/lab6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBB5DC2-69A6-9045-B847-E8B366606D5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67CFAB2-2B8D-C543-A8D5-D72E20EFEE72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" firstSheet="2" activeTab="12" xr2:uid="{49995AF3-CEC5-0640-B888-6C919100F8DC}"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" firstSheet="3" activeTab="13" xr2:uid="{49995AF3-CEC5-0640-B888-6C919100F8DC}"/>
   </bookViews>
   <sheets>
     <sheet name="fore-backward, constant speed" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="roll = 0" sheetId="8" r:id="rId11"/>
     <sheet name="roll = 90" sheetId="12" r:id="rId12"/>
     <sheet name="tapping" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5561" uniqueCount="4271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5563" uniqueCount="4273">
   <si>
     <t>Scaled. Acc (mg) [  00211.91, -00013.18,  00915.53 ], Gyr (DPS) [ -00003.29, -00005.27,  00005.77 ], Mag (uT) [  00485.85, -00103.35, -00316.80 ], Tmp (C) [  00028.84 ]</t>
   </si>
@@ -12858,6 +12859,12 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>yawGyr</t>
+  </si>
+  <si>
+    <t>yawMag</t>
   </si>
 </sst>
 </file>
@@ -21610,7 +21617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDCC34A1-37AD-F84D-9221-930ACC20C7E6}">
   <dimension ref="A1:I506"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -34656,7 +34663,7 @@
         <v>4211</v>
       </c>
       <c r="B451" t="str">
-        <f t="shared" ref="B451:B514" si="43">RIGHT(A451,LEN(A451)-FIND(",",A451)-1)</f>
+        <f t="shared" ref="B451:B506" si="43">RIGHT(A451,LEN(A451)-FIND(",",A451)-1)</f>
         <v>31.25, 997.07, 02192.00</v>
       </c>
       <c r="C451" t="str">
@@ -36273,6 +36280,1533 @@
       <c r="I506" t="str">
         <f t="shared" si="42"/>
         <v>02200.00</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4A85D1-3A75-0443-95AA-FA276F58C031}">
+  <dimension ref="A1:B189"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4271</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5.79</v>
+      </c>
+      <c r="B2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>5.79</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>5.78</v>
+      </c>
+      <c r="B4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5.79</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5.79</v>
+      </c>
+      <c r="B6">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5.79</v>
+      </c>
+      <c r="B7">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5.79</v>
+      </c>
+      <c r="B8">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5.79</v>
+      </c>
+      <c r="B9">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>5.8</v>
+      </c>
+      <c r="B10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>5.81</v>
+      </c>
+      <c r="B11">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5.8</v>
+      </c>
+      <c r="B12">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5.8</v>
+      </c>
+      <c r="B13">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>5.81</v>
+      </c>
+      <c r="B14">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>5.81</v>
+      </c>
+      <c r="B15">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>5.81</v>
+      </c>
+      <c r="B16">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>5.82</v>
+      </c>
+      <c r="B17">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>5.82</v>
+      </c>
+      <c r="B18">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>5.82</v>
+      </c>
+      <c r="B19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>5.82</v>
+      </c>
+      <c r="B20">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>5.84</v>
+      </c>
+      <c r="B21">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>5.83</v>
+      </c>
+      <c r="B22">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>5.83</v>
+      </c>
+      <c r="B23">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>5.83</v>
+      </c>
+      <c r="B24">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>5.83</v>
+      </c>
+      <c r="B25">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>5.82</v>
+      </c>
+      <c r="B26">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>5.82</v>
+      </c>
+      <c r="B27">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>5.83</v>
+      </c>
+      <c r="B28">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>5.82</v>
+      </c>
+      <c r="B29">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>5.82</v>
+      </c>
+      <c r="B30">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>5.83</v>
+      </c>
+      <c r="B31">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>5.82</v>
+      </c>
+      <c r="B32">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>5.82</v>
+      </c>
+      <c r="B33">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>5.83</v>
+      </c>
+      <c r="B34">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>5.83</v>
+      </c>
+      <c r="B35">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>5.83</v>
+      </c>
+      <c r="B36">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>5.82</v>
+      </c>
+      <c r="B37">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>5.83</v>
+      </c>
+      <c r="B38">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>5.84</v>
+      </c>
+      <c r="B39">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>5.84</v>
+      </c>
+      <c r="B40">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>5.84</v>
+      </c>
+      <c r="B41">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>5.85</v>
+      </c>
+      <c r="B42">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>5.85</v>
+      </c>
+      <c r="B43">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>5.84</v>
+      </c>
+      <c r="B44">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>5.86</v>
+      </c>
+      <c r="B45">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>5.86</v>
+      </c>
+      <c r="B46">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>5.86</v>
+      </c>
+      <c r="B47">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>5.86</v>
+      </c>
+      <c r="B48">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>5.86</v>
+      </c>
+      <c r="B49">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>5.86</v>
+      </c>
+      <c r="B50">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>5.85</v>
+      </c>
+      <c r="B51">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>5.86</v>
+      </c>
+      <c r="B52">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>5.86</v>
+      </c>
+      <c r="B53">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>5.87</v>
+      </c>
+      <c r="B54">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>5.87</v>
+      </c>
+      <c r="B55">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>5.87</v>
+      </c>
+      <c r="B56">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>5.87</v>
+      </c>
+      <c r="B57">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>5.87</v>
+      </c>
+      <c r="B58">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>5.87</v>
+      </c>
+      <c r="B59">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>5.88</v>
+      </c>
+      <c r="B60">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>5.88</v>
+      </c>
+      <c r="B61">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>5.88</v>
+      </c>
+      <c r="B62">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>5.87</v>
+      </c>
+      <c r="B63">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>5.87</v>
+      </c>
+      <c r="B64">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>5.87</v>
+      </c>
+      <c r="B65">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>5.87</v>
+      </c>
+      <c r="B66">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>5.87</v>
+      </c>
+      <c r="B67">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>5.87</v>
+      </c>
+      <c r="B68">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>5.87</v>
+      </c>
+      <c r="B69">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>5.87</v>
+      </c>
+      <c r="B70">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>5.88</v>
+      </c>
+      <c r="B71">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>5.88</v>
+      </c>
+      <c r="B72">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>5.88</v>
+      </c>
+      <c r="B73">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>5.88</v>
+      </c>
+      <c r="B74">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>5.88</v>
+      </c>
+      <c r="B75">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>5.88</v>
+      </c>
+      <c r="B76">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>5.88</v>
+      </c>
+      <c r="B77">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>5.88</v>
+      </c>
+      <c r="B78">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>5.88</v>
+      </c>
+      <c r="B79">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>5.88</v>
+      </c>
+      <c r="B80">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>5.88</v>
+      </c>
+      <c r="B81">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>5.89</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>5.89</v>
+      </c>
+      <c r="B83">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>5.89</v>
+      </c>
+      <c r="B84">
+        <v>-0.17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>5.88</v>
+      </c>
+      <c r="B85">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>5.88</v>
+      </c>
+      <c r="B86">
+        <v>-0.15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>5.89</v>
+      </c>
+      <c r="B87">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>5.89</v>
+      </c>
+      <c r="B88">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>5.88</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>5.9</v>
+      </c>
+      <c r="B90">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>5.9</v>
+      </c>
+      <c r="B91">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>5.9</v>
+      </c>
+      <c r="B92">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>5.9</v>
+      </c>
+      <c r="B93">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>5.9</v>
+      </c>
+      <c r="B94">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>5.9</v>
+      </c>
+      <c r="B95">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>5.91</v>
+      </c>
+      <c r="B96">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>5.91</v>
+      </c>
+      <c r="B97">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>5.92</v>
+      </c>
+      <c r="B98">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>5.92</v>
+      </c>
+      <c r="B99">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>5.92</v>
+      </c>
+      <c r="B100">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>5.92</v>
+      </c>
+      <c r="B101">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>5.93</v>
+      </c>
+      <c r="B102">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>5.93</v>
+      </c>
+      <c r="B103">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>5.92</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>5.92</v>
+      </c>
+      <c r="B105">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>5.92</v>
+      </c>
+      <c r="B106">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>5.93</v>
+      </c>
+      <c r="B107">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>5.92</v>
+      </c>
+      <c r="B108">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>5.93</v>
+      </c>
+      <c r="B109">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>5.93</v>
+      </c>
+      <c r="B110">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>5.93</v>
+      </c>
+      <c r="B111">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>5.92</v>
+      </c>
+      <c r="B112">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>5.92</v>
+      </c>
+      <c r="B113">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>5.92</v>
+      </c>
+      <c r="B114">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>5.92</v>
+      </c>
+      <c r="B115">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>5.92</v>
+      </c>
+      <c r="B116">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>5.92</v>
+      </c>
+      <c r="B117">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>5.92</v>
+      </c>
+      <c r="B118">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>5.92</v>
+      </c>
+      <c r="B119">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>5.93</v>
+      </c>
+      <c r="B120">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>5.92</v>
+      </c>
+      <c r="B121">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>5.92</v>
+      </c>
+      <c r="B122">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>5.92</v>
+      </c>
+      <c r="B123">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>5.92</v>
+      </c>
+      <c r="B124">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>5.92</v>
+      </c>
+      <c r="B125">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>5.92</v>
+      </c>
+      <c r="B126">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>5.92</v>
+      </c>
+      <c r="B127">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>5.92</v>
+      </c>
+      <c r="B128">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>5.92</v>
+      </c>
+      <c r="B129">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>5.93</v>
+      </c>
+      <c r="B130">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>5.93</v>
+      </c>
+      <c r="B131">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>5.92</v>
+      </c>
+      <c r="B132">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>5.93</v>
+      </c>
+      <c r="B133">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>5.93</v>
+      </c>
+      <c r="B134">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>5.94</v>
+      </c>
+      <c r="B135">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>5.94</v>
+      </c>
+      <c r="B136">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>5.94</v>
+      </c>
+      <c r="B137">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>5.94</v>
+      </c>
+      <c r="B138">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>5.94</v>
+      </c>
+      <c r="B139">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>5.94</v>
+      </c>
+      <c r="B140">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>5.94</v>
+      </c>
+      <c r="B141">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>5.94</v>
+      </c>
+      <c r="B142">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>5.95</v>
+      </c>
+      <c r="B143">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>5.96</v>
+      </c>
+      <c r="B144">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>5.96</v>
+      </c>
+      <c r="B145">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>5.96</v>
+      </c>
+      <c r="B146">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>5.96</v>
+      </c>
+      <c r="B147">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>5.96</v>
+      </c>
+      <c r="B148">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>5.96</v>
+      </c>
+      <c r="B149">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>5.95</v>
+      </c>
+      <c r="B150">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>5.96</v>
+      </c>
+      <c r="B151">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>5.97</v>
+      </c>
+      <c r="B152">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>5.96</v>
+      </c>
+      <c r="B153">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>5.97</v>
+      </c>
+      <c r="B154">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>5.98</v>
+      </c>
+      <c r="B155">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>5.97</v>
+      </c>
+      <c r="B156">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>5.98</v>
+      </c>
+      <c r="B157">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>5.98</v>
+      </c>
+      <c r="B158">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>5.99</v>
+      </c>
+      <c r="B159">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>5.99</v>
+      </c>
+      <c r="B160">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>5.99</v>
+      </c>
+      <c r="B161">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>5.99</v>
+      </c>
+      <c r="B162">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>5.99</v>
+      </c>
+      <c r="B163">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>5.99</v>
+      </c>
+      <c r="B164">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>5.99</v>
+      </c>
+      <c r="B165">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>5.99</v>
+      </c>
+      <c r="B166">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>6</v>
+      </c>
+      <c r="B167">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>6</v>
+      </c>
+      <c r="B168">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>6</v>
+      </c>
+      <c r="B169">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>6</v>
+      </c>
+      <c r="B170">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>6</v>
+      </c>
+      <c r="B171">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>6.01</v>
+      </c>
+      <c r="B172">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>6.01</v>
+      </c>
+      <c r="B173">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>6.01</v>
+      </c>
+      <c r="B174">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>6.01</v>
+      </c>
+      <c r="B175">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>6.01</v>
+      </c>
+      <c r="B176">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>6.02</v>
+      </c>
+      <c r="B177">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>6.02</v>
+      </c>
+      <c r="B178">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>6.02</v>
+      </c>
+      <c r="B179">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>6.02</v>
+      </c>
+      <c r="B180">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>6.02</v>
+      </c>
+      <c r="B181">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>6.02</v>
+      </c>
+      <c r="B182">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>6.02</v>
+      </c>
+      <c r="B183">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>6.01</v>
+      </c>
+      <c r="B184">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>6.02</v>
+      </c>
+      <c r="B185">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>6.02</v>
+      </c>
+      <c r="B186">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>6.03</v>
+      </c>
+      <c r="B187">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>6.03</v>
+      </c>
+      <c r="B188">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>6.03</v>
+      </c>
+      <c r="B189">
+        <v>0.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>